<commit_message>
feat: add new html
</commit_message>
<xml_diff>
--- a/output/excel/filled_ACTA DE ENTREGA DEL CARNET CON DESCUENTO.xlsx
+++ b/output/excel/filled_ACTA DE ENTREGA DEL CARNET CON DESCUENTO.xlsx
@@ -1771,7 +1771,7 @@
       </c>
       <c r="C7" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Incidunt ut aute ut </t>
+          <t xml:space="preserve">Qui sint nemo in vol </t>
         </is>
       </c>
       <c r="D7" s="12" t="n"/>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="C8" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Qui totam ea at cons </t>
+          <t xml:space="preserve">A fugiat aute nesci </t>
         </is>
       </c>
       <c r="D8" s="12" t="n"/>
@@ -1810,7 +1810,7 @@
     <row r="11">
       <c r="B11" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yo, Consectetur qui qua certifico haber recibido el carnet de identificación como Servidor de la Empresa y a la vez me responsabilizo por el buen uso del mismo y en caso de la finalización de la relación laboral a la devolución del mismo. 
+          <t xml:space="preserve">Yo, Et eiusmod odit ad q certifico haber recibido el carnet de identificación como Servidor de la Empresa y a la vez me responsabilizo por el buen uso del mismo y en caso de la finalización de la relación laboral a la devolución del mismo. 
 Libre y voluntariamente me comprometo a depositar en la cuenta de la Empresa Eléctrica Regional Centro Sur C.A.  el valor de 10usd, correspodiente a la reposición por pérdida del carnet de identificación que he recibido. </t>
         </is>
       </c>
@@ -1870,22 +1870,22 @@
     <row r="17" ht="67" customHeight="1">
       <c r="B17" s="23" t="inlineStr">
         <is>
-          <t xml:space="preserve">27 de febrero de 2008 </t>
+          <t xml:space="preserve">23 de octubre de 2020 </t>
         </is>
       </c>
       <c r="C17" s="24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Non modi maxime exer </t>
+          <t xml:space="preserve">Consequatur numquam  </t>
         </is>
       </c>
       <c r="D17" s="61" t="inlineStr">
         <is>
-          <t xml:space="preserve">At ut sapiente eu la </t>
+          <t xml:space="preserve">Quidem quidem placea </t>
         </is>
       </c>
       <c r="E17" s="24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cupidatat quisquam s </t>
+          <t xml:space="preserve">Ea quas non sit haru </t>
         </is>
       </c>
       <c r="F17" s="25" t="n"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D22" s="27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Soluta et consequunt </t>
+          <t xml:space="preserve">Et vel est nulla aut </t>
         </is>
       </c>
       <c r="E22" s="28" t="n"/>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="D23" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">27 de febrero de 2008 </t>
+          <t xml:space="preserve">23 de octubre de 2020 </t>
         </is>
       </c>
       <c r="E23" s="28" t="n"/>

</xml_diff>

<commit_message>
fix:update templates to generate report
</commit_message>
<xml_diff>
--- a/output/excel/filled_ACTA DE ENTREGA DEL CARNET CON DESCUENTO.xlsx
+++ b/output/excel/filled_ACTA DE ENTREGA DEL CARNET CON DESCUENTO.xlsx
@@ -401,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -605,8 +605,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1769,9 +1775,9 @@
           <t>CIUDAD:</t>
         </is>
       </c>
-      <c r="C7" s="11" t="inlineStr">
+      <c r="C7" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Qui sint nemo in vol </t>
+          <t xml:space="preserve">Recusandae Anim dol </t>
         </is>
       </c>
       <c r="D7" s="12" t="n"/>
@@ -1784,9 +1790,9 @@
           <t>DIRECCIÓN:</t>
         </is>
       </c>
-      <c r="C8" s="11" t="inlineStr">
+      <c r="C8" s="73" t="inlineStr">
         <is>
-          <t xml:space="preserve">A fugiat aute nesci </t>
+          <t xml:space="preserve">Est quis sunt animi </t>
         </is>
       </c>
       <c r="D8" s="12" t="n"/>
@@ -1808,9 +1814,9 @@
       <c r="F10" s="53" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="73" t="inlineStr">
+      <c r="B11" s="74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yo, Et eiusmod odit ad q certifico haber recibido el carnet de identificación como Servidor de la Empresa y a la vez me responsabilizo por el buen uso del mismo y en caso de la finalización de la relación laboral a la devolución del mismo. 
+          <t xml:space="preserve">Yo, Ratione voluptatem hRatione voluptatem hRatione voluptatem h certifico haber recibido el carnet de identificación como Servidor de la Empresa y a la vez me responsabilizo por el buen uso del mismo y en caso de la finalización de la relación laboral a la devolución del mismo. 
 Libre y voluntariamente me comprometo a depositar en la cuenta de la Empresa Eléctrica Regional Centro Sur C.A.  el valor de 10usd, correspodiente a la reposición por pérdida del carnet de identificación que he recibido. </t>
         </is>
       </c>
@@ -1868,24 +1874,24 @@
       </c>
     </row>
     <row r="17" ht="67" customHeight="1">
-      <c r="B17" s="23" t="inlineStr">
+      <c r="B17" s="75" t="inlineStr">
         <is>
-          <t xml:space="preserve">23 de octubre de 2020 </t>
+          <t xml:space="preserve">2 de mayo de 1987 </t>
         </is>
       </c>
       <c r="C17" s="24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Consequatur numquam  </t>
+          <t xml:space="preserve">A aut quod voluptas  </t>
         </is>
       </c>
-      <c r="D17" s="61" t="inlineStr">
+      <c r="D17" s="24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Quidem quidem placea </t>
+          <t xml:space="preserve">Dignissimos voluptat </t>
         </is>
       </c>
       <c r="E17" s="24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ea quas non sit haru </t>
+          <t xml:space="preserve">In tempor exercitati </t>
         </is>
       </c>
       <c r="F17" s="25" t="n"/>
@@ -1927,7 +1933,7 @@
       </c>
       <c r="D22" s="27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Et vel est nulla aut </t>
+          <t xml:space="preserve">Non cillum molestiae </t>
         </is>
       </c>
       <c r="E22" s="28" t="n"/>
@@ -1942,7 +1948,7 @@
       </c>
       <c r="D23" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">23 de octubre de 2020 </t>
+          <t xml:space="preserve">2 de mayo de 1987 </t>
         </is>
       </c>
       <c r="E23" s="28" t="n"/>

</xml_diff>